<commit_message>
updated zero shot and other changes
</commit_message>
<xml_diff>
--- a/Data_ML_cleaned.xlsx
+++ b/Data_ML_cleaned.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P110"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,25 +495,10 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>result_clean</t>
+          <t>split_info</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>split_info</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>initiative_short</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>text_length</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>doc_len</t>
         </is>
@@ -567,23 +552,10 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Für den Schutz vor Waffengewalt</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
-        <v>2261</v>
-      </c>
-      <c r="P2" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
         <v>162</v>
       </c>
     </row>
@@ -635,23 +607,10 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Für den Schutz vor Waffengewalt</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
-        <v>2263</v>
-      </c>
-      <c r="P3" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
         <v>132</v>
       </c>
     </row>
@@ -703,23 +662,10 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Für den Schutz vor Waffengewalt</t>
-        </is>
-      </c>
-      <c r="O4" t="n">
-        <v>1911</v>
-      </c>
-      <c r="P4" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
         <v>120</v>
       </c>
     </row>
@@ -770,23 +716,10 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Für den Schutz vor Waffengewalt</t>
-        </is>
-      </c>
-      <c r="O5" t="n">
-        <v>1804</v>
-      </c>
-      <c r="P5" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
         <v>121</v>
       </c>
     </row>
@@ -837,23 +770,10 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Für den Schutz vor Waffengewalt</t>
-        </is>
-      </c>
-      <c r="O6" t="n">
-        <v>1096</v>
-      </c>
-      <c r="P6" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
         <v>71</v>
       </c>
     </row>
@@ -903,23 +823,10 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Gegen Masseneinwanderung</t>
-        </is>
-      </c>
-      <c r="O7" t="n">
-        <v>3968</v>
-      </c>
-      <c r="P7" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
         <v>254</v>
       </c>
     </row>
@@ -965,23 +872,10 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Gegen Masseneinwanderung</t>
-        </is>
-      </c>
-      <c r="O8" t="n">
-        <v>6501</v>
-      </c>
-      <c r="P8" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
         <v>414</v>
       </c>
     </row>
@@ -1033,23 +927,10 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Gegen Masseneinwanderung</t>
-        </is>
-      </c>
-      <c r="O9" t="n">
-        <v>2097</v>
-      </c>
-      <c r="P9" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
         <v>127</v>
       </c>
     </row>
@@ -1101,23 +982,10 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Gegen Masseneinwanderung</t>
-        </is>
-      </c>
-      <c r="O10" t="n">
-        <v>1887</v>
-      </c>
-      <c r="P10" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
         <v>113</v>
       </c>
     </row>
@@ -1169,23 +1037,10 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>Gegen Masseneinwanderung</t>
-        </is>
-      </c>
-      <c r="O11" t="n">
-        <v>4336</v>
-      </c>
-      <c r="P11" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
         <v>261</v>
       </c>
     </row>
@@ -1237,23 +1092,10 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>Gegen Masseneinwanderung</t>
-        </is>
-      </c>
-      <c r="O12" t="n">
-        <v>2516</v>
-      </c>
-      <c r="P12" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
         <v>161</v>
       </c>
     </row>
@@ -1305,23 +1147,10 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>Gegen Masseneinwanderung</t>
-        </is>
-      </c>
-      <c r="O13" t="n">
-        <v>5066</v>
-      </c>
-      <c r="P13" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
         <v>333</v>
       </c>
     </row>
@@ -1373,23 +1202,10 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Pädophilen-Initiative</t>
-        </is>
-      </c>
-      <c r="O14" t="n">
-        <v>4543</v>
-      </c>
-      <c r="P14" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
         <v>294</v>
       </c>
     </row>
@@ -1441,23 +1257,10 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>Pädophilen-Initiative</t>
-        </is>
-      </c>
-      <c r="O15" t="n">
-        <v>5945</v>
-      </c>
-      <c r="P15" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
         <v>395</v>
       </c>
     </row>
@@ -1509,23 +1312,10 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>Pädophilen-Initiative</t>
-        </is>
-      </c>
-      <c r="O16" t="n">
-        <v>3274</v>
-      </c>
-      <c r="P16" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
         <v>207</v>
       </c>
     </row>
@@ -1577,23 +1367,10 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>Pädophilen-Initiative</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>3548</v>
-      </c>
-      <c r="P17" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
         <v>226</v>
       </c>
     </row>
@@ -1645,23 +1422,10 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>Pädophilen-Initiative</t>
-        </is>
-      </c>
-      <c r="O18" t="n">
-        <v>1373</v>
-      </c>
-      <c r="P18" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
         <v>88</v>
       </c>
     </row>
@@ -1732,23 +1496,10 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>Erbschaftssteuerreform</t>
-        </is>
-      </c>
-      <c r="O19" t="n">
-        <v>4536</v>
-      </c>
-      <c r="P19" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
         <v>297</v>
       </c>
     </row>
@@ -1808,23 +1559,10 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>Erbschaftssteuerreform</t>
-        </is>
-      </c>
-      <c r="O20" t="n">
-        <v>2591</v>
-      </c>
-      <c r="P20" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
         <v>173</v>
       </c>
     </row>
@@ -1876,23 +1614,10 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>Erbschaftssteuerreform</t>
-        </is>
-      </c>
-      <c r="O21" t="n">
-        <v>2970</v>
-      </c>
-      <c r="P21" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
         <v>185</v>
       </c>
     </row>
@@ -1944,23 +1669,10 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>Erbschaftssteuerreform</t>
-        </is>
-      </c>
-      <c r="O22" t="n">
-        <v>4574</v>
-      </c>
-      <c r="P22" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2012,23 +1724,10 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>Erbschaftssteuerreform</t>
-        </is>
-      </c>
-      <c r="O23" t="n">
-        <v>3488</v>
-      </c>
-      <c r="P23" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
         <v>220</v>
       </c>
     </row>
@@ -2080,23 +1779,10 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>Erbschaftssteuerreform</t>
-        </is>
-      </c>
-      <c r="O24" t="n">
-        <v>4126</v>
-      </c>
-      <c r="P24" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
         <v>270</v>
       </c>
     </row>
@@ -2157,23 +1843,10 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>Abschaffung der Billag-Gebühren</t>
-        </is>
-      </c>
-      <c r="O25" t="n">
-        <v>6701</v>
-      </c>
-      <c r="P25" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
         <v>423</v>
       </c>
     </row>
@@ -2229,23 +1902,10 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>Abschaffung der Billag-Gebühren</t>
-        </is>
-      </c>
-      <c r="O26" t="n">
-        <v>3219</v>
-      </c>
-      <c r="P26" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
         <v>203</v>
       </c>
     </row>
@@ -2297,23 +1957,10 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>Abschaffung der Billag-Gebühren</t>
-        </is>
-      </c>
-      <c r="O27" t="n">
-        <v>3593</v>
-      </c>
-      <c r="P27" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
         <v>232</v>
       </c>
     </row>
@@ -2365,23 +2012,10 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>Abschaffung der Billag-Gebühren</t>
-        </is>
-      </c>
-      <c r="O28" t="n">
-        <v>2379</v>
-      </c>
-      <c r="P28" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
         <v>160</v>
       </c>
     </row>
@@ -2433,23 +2067,10 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>Abschaffung der Billag-Gebühren</t>
-        </is>
-      </c>
-      <c r="O29" t="n">
-        <v>4079</v>
-      </c>
-      <c r="P29" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
         <v>259</v>
       </c>
     </row>
@@ -2504,23 +2125,10 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>Hornkuh-Initiative</t>
-        </is>
-      </c>
-      <c r="O30" t="n">
-        <v>2872</v>
-      </c>
-      <c r="P30" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
         <v>191</v>
       </c>
     </row>
@@ -2580,23 +2188,10 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>Hornkuh-Initiative</t>
-        </is>
-      </c>
-      <c r="O31" t="n">
-        <v>4370</v>
-      </c>
-      <c r="P31" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
         <v>295</v>
       </c>
     </row>
@@ -2650,23 +2245,10 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>Hornkuh-Initiative</t>
-        </is>
-      </c>
-      <c r="O32" t="n">
-        <v>2262</v>
-      </c>
-      <c r="P32" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
         <v>156</v>
       </c>
     </row>
@@ -2718,23 +2300,10 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>Hornkuh-Initiative</t>
-        </is>
-      </c>
-      <c r="O33" t="n">
-        <v>2854</v>
-      </c>
-      <c r="P33" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
         <v>185</v>
       </c>
     </row>
@@ -2786,23 +2355,10 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>Selbstbestimmungsinitiative</t>
-        </is>
-      </c>
-      <c r="O34" t="n">
-        <v>3687</v>
-      </c>
-      <c r="P34" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
         <v>234</v>
       </c>
     </row>
@@ -2854,23 +2410,10 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>Selbstbestimmungsinitiative</t>
-        </is>
-      </c>
-      <c r="O35" t="n">
-        <v>5644</v>
-      </c>
-      <c r="P35" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
         <v>361</v>
       </c>
     </row>
@@ -2928,23 +2471,10 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>Selbstbestimmungsinitiative</t>
-        </is>
-      </c>
-      <c r="O36" t="n">
-        <v>3739</v>
-      </c>
-      <c r="P36" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
         <v>230</v>
       </c>
     </row>
@@ -3024,23 +2554,10 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>Selbstbestimmungsinitiative</t>
-        </is>
-      </c>
-      <c r="O37" t="n">
-        <v>12067</v>
-      </c>
-      <c r="P37" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
         <v>745</v>
       </c>
     </row>
@@ -3092,23 +2609,10 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>Selbstbestimmungsinitiative</t>
-        </is>
-      </c>
-      <c r="O38" t="n">
-        <v>1559</v>
-      </c>
-      <c r="P38" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
         <v>102</v>
       </c>
     </row>
@@ -3160,23 +2664,10 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>Begrenzungsinitiative</t>
-        </is>
-      </c>
-      <c r="O39" t="n">
-        <v>4397</v>
-      </c>
-      <c r="P39" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
         <v>282</v>
       </c>
     </row>
@@ -3228,23 +2719,10 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>Begrenzungsinitiative</t>
-        </is>
-      </c>
-      <c r="O40" t="n">
-        <v>1671</v>
-      </c>
-      <c r="P40" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
         <v>100</v>
       </c>
     </row>
@@ -3296,23 +2774,10 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>Begrenzungsinitiative</t>
-        </is>
-      </c>
-      <c r="O41" t="n">
-        <v>5672</v>
-      </c>
-      <c r="P41" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
         <v>354</v>
       </c>
     </row>
@@ -3387,23 +2852,10 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>Begrenzungsinitiative</t>
-        </is>
-      </c>
-      <c r="O42" t="n">
-        <v>9754</v>
-      </c>
-      <c r="P42" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
         <v>615</v>
       </c>
     </row>
@@ -3455,23 +2907,10 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>Begrenzungsinitiative</t>
-        </is>
-      </c>
-      <c r="O43" t="n">
-        <v>2420</v>
-      </c>
-      <c r="P43" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
         <v>149</v>
       </c>
     </row>
@@ -3523,23 +2962,10 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>Begrenzungsinitiative</t>
-        </is>
-      </c>
-      <c r="O44" t="n">
-        <v>3520</v>
-      </c>
-      <c r="P44" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
         <v>210</v>
       </c>
     </row>
@@ -3591,23 +3017,10 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>Konzernverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O45" t="n">
-        <v>2962</v>
-      </c>
-      <c r="P45" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
         <v>185</v>
       </c>
     </row>
@@ -3659,23 +3072,10 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>Konzernverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O46" t="n">
-        <v>2240</v>
-      </c>
-      <c r="P46" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
         <v>138</v>
       </c>
     </row>
@@ -3741,23 +3141,10 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>Konzernverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O47" t="n">
-        <v>4309</v>
-      </c>
-      <c r="P47" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
         <v>291</v>
       </c>
     </row>
@@ -3825,23 +3212,10 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>Konzernverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O48" t="n">
-        <v>5724</v>
-      </c>
-      <c r="P48" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
         <v>373</v>
       </c>
     </row>
@@ -3893,23 +3267,10 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>Konzernverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O49" t="n">
-        <v>5495</v>
-      </c>
-      <c r="P49" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
         <v>346</v>
       </c>
     </row>
@@ -3961,23 +3322,10 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>Kriegsgeschäft-Initiative</t>
-        </is>
-      </c>
-      <c r="O50" t="n">
-        <v>3715</v>
-      </c>
-      <c r="P50" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
         <v>239</v>
       </c>
     </row>
@@ -4029,23 +3377,10 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>Kriegsgeschäft-Initiative</t>
-        </is>
-      </c>
-      <c r="O51" t="n">
-        <v>3621</v>
-      </c>
-      <c r="P51" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
         <v>239</v>
       </c>
     </row>
@@ -4099,23 +3434,10 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>Kriegsgeschäft-Initiative</t>
-        </is>
-      </c>
-      <c r="O52" t="n">
-        <v>3781</v>
-      </c>
-      <c r="P52" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M52" t="n">
         <v>251</v>
       </c>
     </row>
@@ -4167,23 +3489,10 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>Kriegsgeschäft-Initiative</t>
-        </is>
-      </c>
-      <c r="O53" t="n">
-        <v>3414</v>
-      </c>
-      <c r="P53" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M53" t="n">
         <v>211</v>
       </c>
     </row>
@@ -4246,23 +3555,10 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>Kriegsgeschäft-Initiative</t>
-        </is>
-      </c>
-      <c r="O54" t="n">
-        <v>3122</v>
-      </c>
-      <c r="P54" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M54" t="n">
         <v>208</v>
       </c>
     </row>
@@ -4329,23 +3625,10 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>Kriegsgeschäft-Initiative</t>
-        </is>
-      </c>
-      <c r="O55" t="n">
-        <v>3574</v>
-      </c>
-      <c r="P55" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M55" t="n">
         <v>228</v>
       </c>
     </row>
@@ -4397,23 +3680,10 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>Ja zum Verhüllungsverbot</t>
-        </is>
-      </c>
-      <c r="O56" t="n">
-        <v>2005</v>
-      </c>
-      <c r="P56" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M56" t="n">
         <v>118</v>
       </c>
     </row>
@@ -4465,23 +3735,10 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>Ja zum Verhüllungsverbot</t>
-        </is>
-      </c>
-      <c r="O57" t="n">
-        <v>2027</v>
-      </c>
-      <c r="P57" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M57" t="n">
         <v>128</v>
       </c>
     </row>
@@ -4533,23 +3790,10 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>Ja zum Verhüllungsverbot</t>
-        </is>
-      </c>
-      <c r="O58" t="n">
-        <v>2721</v>
-      </c>
-      <c r="P58" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M58" t="n">
         <v>179</v>
       </c>
     </row>
@@ -4607,23 +3851,10 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>Ja zum Verhüllungsverbot</t>
-        </is>
-      </c>
-      <c r="O59" t="n">
-        <v>2936</v>
-      </c>
-      <c r="P59" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M59" t="n">
         <v>196</v>
       </c>
     </row>
@@ -4703,23 +3934,10 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>Ja zum Verhüllungsverbot</t>
-        </is>
-      </c>
-      <c r="O60" t="n">
-        <v>11076</v>
-      </c>
-      <c r="P60" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M60" t="n">
         <v>687</v>
       </c>
     </row>
@@ -4771,23 +3989,10 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>99%-Initiative</t>
-        </is>
-      </c>
-      <c r="O61" t="n">
-        <v>3727</v>
-      </c>
-      <c r="P61" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
         <v>267</v>
       </c>
     </row>
@@ -4839,23 +4044,10 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>99%-Initiative</t>
-        </is>
-      </c>
-      <c r="O62" t="n">
-        <v>2816</v>
-      </c>
-      <c r="P62" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
         <v>199</v>
       </c>
     </row>
@@ -4907,23 +4099,10 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N63" t="inlineStr">
-        <is>
-          <t>99%-Initiative</t>
-        </is>
-      </c>
-      <c r="O63" t="n">
-        <v>1952</v>
-      </c>
-      <c r="P63" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
         <v>127</v>
       </c>
     </row>
@@ -4975,23 +4154,10 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>99%-Initiative</t>
-        </is>
-      </c>
-      <c r="O64" t="n">
-        <v>2877</v>
-      </c>
-      <c r="P64" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
         <v>181</v>
       </c>
     </row>
@@ -5058,23 +4224,10 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>99%-Initiative</t>
-        </is>
-      </c>
-      <c r="O65" t="n">
-        <v>7842</v>
-      </c>
-      <c r="P65" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
         <v>482</v>
       </c>
     </row>
@@ -5136,23 +4289,10 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>99%-Initiative</t>
-        </is>
-      </c>
-      <c r="O66" t="n">
-        <v>3979</v>
-      </c>
-      <c r="P66" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M66" t="n">
         <v>237</v>
       </c>
     </row>
@@ -5212,23 +4352,10 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>Pflegeinitiative</t>
-        </is>
-      </c>
-      <c r="O67" t="n">
-        <v>3646</v>
-      </c>
-      <c r="P67" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
         <v>201</v>
       </c>
     </row>
@@ -5292,23 +4419,10 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N68" t="inlineStr">
-        <is>
-          <t>Pflegeinitiative</t>
-        </is>
-      </c>
-      <c r="O68" t="n">
-        <v>4155</v>
-      </c>
-      <c r="P68" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M68" t="n">
         <v>257</v>
       </c>
     </row>
@@ -5372,23 +4486,10 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N69" t="inlineStr">
-        <is>
-          <t>Pflegeinitiative</t>
-        </is>
-      </c>
-      <c r="O69" t="n">
-        <v>5299</v>
-      </c>
-      <c r="P69" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
         <v>326</v>
       </c>
     </row>
@@ -5446,23 +4547,10 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>Pflegeinitiative</t>
-        </is>
-      </c>
-      <c r="O70" t="n">
-        <v>2785</v>
-      </c>
-      <c r="P70" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M70" t="n">
         <v>169</v>
       </c>
     </row>
@@ -5514,23 +4602,10 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>Pflegeinitiative</t>
-        </is>
-      </c>
-      <c r="O71" t="n">
-        <v>3495</v>
-      </c>
-      <c r="P71" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M71" t="n">
         <v>220</v>
       </c>
     </row>
@@ -5587,23 +4662,10 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N72" t="inlineStr">
-        <is>
-          <t>Pflegeinitiative</t>
-        </is>
-      </c>
-      <c r="O72" t="n">
-        <v>4116</v>
-      </c>
-      <c r="P72" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M72" t="n">
         <v>265</v>
       </c>
     </row>
@@ -5657,23 +4719,10 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N73" t="inlineStr">
-        <is>
-          <t>Pflegeinitiative</t>
-        </is>
-      </c>
-      <c r="O73" t="n">
-        <v>2539</v>
-      </c>
-      <c r="P73" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
         <v>165</v>
       </c>
     </row>
@@ -5736,23 +4785,10 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N74" t="inlineStr">
-        <is>
-          <t>Justiz-Initiative</t>
-        </is>
-      </c>
-      <c r="O74" t="n">
-        <v>3873</v>
-      </c>
-      <c r="P74" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
         <v>223</v>
       </c>
     </row>
@@ -5804,23 +4840,10 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N75" t="inlineStr">
-        <is>
-          <t>Justiz-Initiative</t>
-        </is>
-      </c>
-      <c r="O75" t="n">
-        <v>3728</v>
-      </c>
-      <c r="P75" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
         <v>246</v>
       </c>
     </row>
@@ -5872,23 +4895,10 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N76" t="inlineStr">
-        <is>
-          <t>Justiz-Initiative</t>
-        </is>
-      </c>
-      <c r="O76" t="n">
-        <v>5406</v>
-      </c>
-      <c r="P76" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
         <v>326</v>
       </c>
     </row>
@@ -5941,23 +4951,10 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N77" t="inlineStr">
-        <is>
-          <t>Justiz-Initiative</t>
-        </is>
-      </c>
-      <c r="O77" t="n">
-        <v>2335</v>
-      </c>
-      <c r="P77" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
         <v>150</v>
       </c>
     </row>
@@ -6009,23 +5006,10 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N78" t="inlineStr">
-        <is>
-          <t>Justiz-Initiative</t>
-        </is>
-      </c>
-      <c r="O78" t="n">
-        <v>3989</v>
-      </c>
-      <c r="P78" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
         <v>247</v>
       </c>
     </row>
@@ -6091,23 +5075,10 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>Tierversuchsverbot-Initiative</t>
-        </is>
-      </c>
-      <c r="O79" t="n">
-        <v>5131</v>
-      </c>
-      <c r="P79" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
         <v>330</v>
       </c>
     </row>
@@ -6161,23 +5132,10 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N80" t="inlineStr">
-        <is>
-          <t>Tierversuchsverbot-Initiative</t>
-        </is>
-      </c>
-      <c r="O80" t="n">
-        <v>4826</v>
-      </c>
-      <c r="P80" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
         <v>304</v>
       </c>
     </row>
@@ -6231,23 +5189,10 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N81" t="inlineStr">
-        <is>
-          <t>Tierversuchsverbot-Initiative</t>
-        </is>
-      </c>
-      <c r="O81" t="n">
-        <v>4069</v>
-      </c>
-      <c r="P81" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
         <v>275</v>
       </c>
     </row>
@@ -6299,23 +5244,10 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N82" t="inlineStr">
-        <is>
-          <t>Tierversuchsverbot-Initiative</t>
-        </is>
-      </c>
-      <c r="O82" t="n">
-        <v>4899</v>
-      </c>
-      <c r="P82" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
         <v>317</v>
       </c>
     </row>
@@ -6380,23 +5312,10 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N83" t="inlineStr">
-        <is>
-          <t>Tierversuchsverbot-Initiative</t>
-        </is>
-      </c>
-      <c r="O83" t="n">
-        <v>4854</v>
-      </c>
-      <c r="P83" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
         <v>291</v>
       </c>
     </row>
@@ -6476,23 +5395,10 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N84" t="inlineStr">
-        <is>
-          <t>Tierversuchsverbot-Initiative</t>
-        </is>
-      </c>
-      <c r="O84" t="n">
-        <v>9244</v>
-      </c>
-      <c r="P84" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
         <v>575</v>
       </c>
     </row>
@@ -6544,23 +5450,10 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N85" t="inlineStr">
-        <is>
-          <t>Massentierhaltungsinitiative</t>
-        </is>
-      </c>
-      <c r="O85" t="n">
-        <v>3666</v>
-      </c>
-      <c r="P85" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
         <v>242</v>
       </c>
     </row>
@@ -6612,23 +5505,10 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N86" t="inlineStr">
-        <is>
-          <t>Massentierhaltungsinitiative</t>
-        </is>
-      </c>
-      <c r="O86" t="n">
-        <v>3630</v>
-      </c>
-      <c r="P86" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
         <v>234</v>
       </c>
     </row>
@@ -6680,23 +5560,10 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>Massentierhaltungsinitiative</t>
-        </is>
-      </c>
-      <c r="O87" t="n">
-        <v>2475</v>
-      </c>
-      <c r="P87" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
         <v>173</v>
       </c>
     </row>
@@ -6748,23 +5615,10 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N88" t="inlineStr">
-        <is>
-          <t>Massentierhaltungsinitiative</t>
-        </is>
-      </c>
-      <c r="O88" t="n">
-        <v>3256</v>
-      </c>
-      <c r="P88" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M88" t="n">
         <v>210</v>
       </c>
     </row>
@@ -6818,23 +5672,10 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t>Massentierhaltungsinitiative</t>
-        </is>
-      </c>
-      <c r="O89" t="n">
-        <v>4025</v>
-      </c>
-      <c r="P89" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
         <v>249</v>
       </c>
     </row>
@@ -6892,23 +5733,10 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>Initiative für eine 13. AHV-Rente</t>
-        </is>
-      </c>
-      <c r="O90" t="n">
-        <v>2707</v>
-      </c>
-      <c r="P90" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
         <v>180</v>
       </c>
     </row>
@@ -6979,23 +5807,10 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N91" t="inlineStr">
-        <is>
-          <t>Initiative für eine 13. AHV-Rente</t>
-        </is>
-      </c>
-      <c r="O91" t="n">
-        <v>7273</v>
-      </c>
-      <c r="P91" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
         <v>478</v>
       </c>
     </row>
@@ -7047,23 +5862,10 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>Initiative für eine 13. AHV-Rente</t>
-        </is>
-      </c>
-      <c r="O92" t="n">
-        <v>4485</v>
-      </c>
-      <c r="P92" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
         <v>316</v>
       </c>
     </row>
@@ -7115,23 +5917,10 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N93" t="inlineStr">
-        <is>
-          <t>Initiative für eine 13. AHV-Rente</t>
-        </is>
-      </c>
-      <c r="O93" t="n">
-        <v>3759</v>
-      </c>
-      <c r="P93" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M93" t="n">
         <v>253</v>
       </c>
     </row>
@@ -7183,23 +5972,10 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>angenommen</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N94" t="inlineStr">
-        <is>
-          <t>Initiative für eine 13. AHV-Rente</t>
-        </is>
-      </c>
-      <c r="O94" t="n">
-        <v>3368</v>
-      </c>
-      <c r="P94" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
         <v>226</v>
       </c>
     </row>
@@ -7251,23 +6027,10 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N95" t="inlineStr">
-        <is>
-          <t>Kostenbremse-Initiative</t>
-        </is>
-      </c>
-      <c r="O95" t="n">
-        <v>3040</v>
-      </c>
-      <c r="P95" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
         <v>207</v>
       </c>
     </row>
@@ -7319,23 +6082,10 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N96" t="inlineStr">
-        <is>
-          <t>Kostenbremse-Initiative</t>
-        </is>
-      </c>
-      <c r="O96" t="n">
-        <v>2623</v>
-      </c>
-      <c r="P96" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M96" t="n">
         <v>182</v>
       </c>
     </row>
@@ -7389,23 +6139,10 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N97" t="inlineStr">
-        <is>
-          <t>Kostenbremse-Initiative</t>
-        </is>
-      </c>
-      <c r="O97" t="n">
-        <v>3381</v>
-      </c>
-      <c r="P97" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M97" t="n">
         <v>210</v>
       </c>
     </row>
@@ -7457,23 +6194,10 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N98" t="inlineStr">
-        <is>
-          <t>Kostenbremse-Initiative</t>
-        </is>
-      </c>
-      <c r="O98" t="n">
-        <v>5572</v>
-      </c>
-      <c r="P98" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M98" t="n">
         <v>355</v>
       </c>
     </row>
@@ -7542,23 +6266,10 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N99" t="inlineStr">
-        <is>
-          <t>Kostenbremse-Initiative</t>
-        </is>
-      </c>
-      <c r="O99" t="n">
-        <v>8105</v>
-      </c>
-      <c r="P99" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M99" t="n">
         <v>501</v>
       </c>
     </row>
@@ -7620,23 +6331,10 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N100" t="inlineStr">
-        <is>
-          <t>Biodiversitätsinitiative</t>
-        </is>
-      </c>
-      <c r="O100" t="n">
-        <v>4271</v>
-      </c>
-      <c r="P100" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M100" t="n">
         <v>274</v>
       </c>
     </row>
@@ -7703,23 +6401,10 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N101" t="inlineStr">
-        <is>
-          <t>Biodiversitätsinitiative</t>
-        </is>
-      </c>
-      <c r="O101" t="n">
-        <v>5696</v>
-      </c>
-      <c r="P101" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M101" t="n">
         <v>356</v>
       </c>
     </row>
@@ -7771,23 +6456,10 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N102" t="inlineStr">
-        <is>
-          <t>Biodiversitätsinitiative</t>
-        </is>
-      </c>
-      <c r="O102" t="n">
-        <v>4387</v>
-      </c>
-      <c r="P102" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M102" t="n">
         <v>268</v>
       </c>
     </row>
@@ -7839,23 +6511,10 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N103" t="inlineStr">
-        <is>
-          <t>Biodiversitätsinitiative</t>
-        </is>
-      </c>
-      <c r="O103" t="n">
-        <v>4937</v>
-      </c>
-      <c r="P103" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M103" t="n">
         <v>322</v>
       </c>
     </row>
@@ -7909,23 +6568,10 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N104" t="inlineStr">
-        <is>
-          <t>Biodiversitätsinitiative</t>
-        </is>
-      </c>
-      <c r="O104" t="n">
-        <v>3754</v>
-      </c>
-      <c r="P104" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M104" t="n">
         <v>229</v>
       </c>
     </row>
@@ -7981,23 +6627,10 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N105" t="inlineStr">
-        <is>
-          <t>Umweltverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O105" t="n">
-        <v>1326</v>
-      </c>
-      <c r="P105" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M105" t="n">
         <v>94</v>
       </c>
     </row>
@@ -8071,23 +6704,10 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N106" t="inlineStr">
-        <is>
-          <t>Umweltverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O106" t="n">
-        <v>7825</v>
-      </c>
-      <c r="P106" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M106" t="n">
         <v>504</v>
       </c>
     </row>
@@ -8157,23 +6777,10 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N107" t="inlineStr">
-        <is>
-          <t>Umweltverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O107" t="n">
-        <v>7117</v>
-      </c>
-      <c r="P107" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M107" t="n">
         <v>479</v>
       </c>
     </row>
@@ -8225,23 +6832,10 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M108" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N108" t="inlineStr">
-        <is>
-          <t>Umweltverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O108" t="n">
-        <v>4332</v>
-      </c>
-      <c r="P108" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M108" t="n">
         <v>294</v>
       </c>
     </row>
@@ -8293,23 +6887,10 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N109" t="inlineStr">
-        <is>
-          <t>Umweltverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O109" t="n">
-        <v>6926</v>
-      </c>
-      <c r="P109" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M109" t="n">
         <v>457</v>
       </c>
     </row>
@@ -8363,23 +6944,10 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
-        </is>
-      </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="N110" t="inlineStr">
-        <is>
-          <t>Umweltverantwortungsinitiative</t>
-        </is>
-      </c>
-      <c r="O110" t="n">
-        <v>2494</v>
-      </c>
-      <c r="P110" t="n">
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M110" t="n">
         <v>161</v>
       </c>
     </row>

</xml_diff>